<commit_message>
Add citation file and newer version of test
</commit_message>
<xml_diff>
--- a/results/cicddos2019-gnb-results.xlsx
+++ b/results/cicddos2019-gnb-results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,37 +466,72 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>accuracy</t>
+          <t>accuracy_lvl_1</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>recall_0</t>
+          <t>recall_0_lvl_1</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>recall_1</t>
+          <t>recall_1_lvl_1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>precision_0</t>
+          <t>precision_0_lvl_1</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>precision_1</t>
+          <t>precision_1_lvl_1</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>f1_score_0</t>
+          <t>f1_score_0_lvl_1</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>f1_score_1</t>
+          <t>f1_score_1_lvl_1</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_lvl_2</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>recall_0_lvl_2</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>recall_1_lvl_2</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>precision_0_lvl_2</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>precision_1_lvl_2</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>f1_score_0_lvl_2</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>f1_score_1_lvl_2</t>
         </is>
       </c>
     </row>
@@ -511,7 +546,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -524,13 +559,13 @@
         <v>30</v>
       </c>
       <c r="G2" t="n">
-        <v>41902</v>
+        <v>40450</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9550856761013794</v>
+        <v>0.9614833127317676</v>
       </c>
       <c r="I2" t="n">
-        <v>0.764632316158079</v>
+        <v>0.6308056872037915</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
@@ -539,13 +574,34 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9474125405163742</v>
+        <v>0.9587699798877951</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8666194188518781</v>
+        <v>0.7736123219994188</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9729962407093867</v>
+        <v>0.9789510659569294</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.961557478368356</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.6315165876777251</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.9588461029509064</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.7741466957153231</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.9789907451192327</v>
       </c>
     </row>
     <row r="3">
@@ -559,7 +615,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -572,13 +628,13 @@
         <v>60</v>
       </c>
       <c r="G3" t="n">
-        <v>42274</v>
+        <v>40410</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9464446231726357</v>
+        <v>0.9524870081662955</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7451598379108509</v>
+        <v>0.5801443253881479</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -587,13 +643,34 @@
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9365008133729735</v>
+        <v>0.9491485022644808</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8539731682146542</v>
+        <v>0.7342928314420151</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9672093157986211</v>
+        <v>0.973910916650814</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.952585993565949</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.5810190247102559</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.9492490662993669</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.7349930843706777</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.9739638537844816</v>
       </c>
     </row>
     <row r="4">
@@ -607,7 +684,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -620,13 +697,13 @@
         <v>120</v>
       </c>
       <c r="G4" t="n">
-        <v>41881</v>
+        <v>40289</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9489983524748693</v>
+        <v>0.9569361364144059</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7432075018033181</v>
+        <v>0.6005985267034991</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -635,13 +712,34 @@
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9401663912154402</v>
+        <v>0.9539543524416136</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8526896551724138</v>
+        <v>0.7504674241334676</v>
       </c>
       <c r="N4" t="n">
-        <v>0.9691605786722879</v>
+        <v>0.9764346349745331</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.9571595224502966</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.602670349907919</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.954182262217621</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.7520827348463086</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.9765540099978266</v>
       </c>
     </row>
     <row r="5">
@@ -655,7 +753,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -668,13 +766,13 @@
         <v>180</v>
       </c>
       <c r="G5" t="n">
-        <v>41793</v>
+        <v>40087</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9474792429354199</v>
+        <v>0.9582158804599995</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7428537956888472</v>
+        <v>0.6142330723169046</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
@@ -683,13 +781,34 @@
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9380852984316823</v>
+        <v>0.955237840726884</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8524568125294079</v>
+        <v>0.7610215437294907</v>
       </c>
       <c r="N5" t="n">
-        <v>0.9680536756465674</v>
+        <v>0.9771065400123009</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.9583156634320353</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.6151543067710732</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.9553399615137909</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.7617282190218166</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.9771599622749826</v>
       </c>
     </row>
     <row r="6">
@@ -703,7 +822,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -716,13 +835,13 @@
         <v>240</v>
       </c>
       <c r="G6" t="n">
-        <v>41221</v>
+        <v>39819</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9477450813905534</v>
+        <v>0.9601195409226752</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7208036292935839</v>
+        <v>0.6023040320560982</v>
       </c>
       <c r="J6" t="n">
         <v>1</v>
@@ -731,13 +850,34 @@
         <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9395961862030286</v>
+        <v>0.9575559950820548</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8377523350406748</v>
+        <v>0.7517974366989685</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9688575311569269</v>
+        <v>0.9783178590933916</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.96016976820111</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.6028049085900326</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.9576071848604726</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.7521875</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.978344575220514</v>
       </c>
     </row>
     <row r="7">
@@ -751,7 +891,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -764,13 +904,13 @@
         <v>300</v>
       </c>
       <c r="G7" t="n">
-        <v>41422</v>
+        <v>39690</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9527304331031818</v>
+        <v>0.9556059460821366</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7647482878769675</v>
+        <v>0.5881252921926133</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -779,13 +919,34 @@
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>0.944148101663006</v>
+        <v>0.952601280464841</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8666938997821351</v>
+        <v>0.7406535178098321</v>
       </c>
       <c r="N7" t="n">
-        <v>0.9712717882504842</v>
+        <v>0.9757253464855481</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.9557319223985891</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.5892940626460963</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.9527294250585165</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.7415796440653037</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.9757925627919153</v>
       </c>
     </row>
     <row r="8">
@@ -799,7 +960,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -812,13 +973,13 @@
         <v>30</v>
       </c>
       <c r="G8" t="n">
-        <v>42044</v>
+        <v>40550</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9750499476738654</v>
+        <v>0.9750924784217017</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8728330706752334</v>
+        <v>0.775355871886121</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
@@ -827,13 +988,34 @@
         <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9698943864079899</v>
+        <v>0.9727498381178502</v>
       </c>
       <c r="M8" t="n">
-        <v>0.9320991649944981</v>
+        <v>0.8734652969180657</v>
       </c>
       <c r="N8" t="n">
-        <v>0.9847171433150249</v>
+        <v>0.986186711890369</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.9751418002466091</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.7758007117437722</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.9728023312287518</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.8737474949899799</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.9862136878385033</v>
       </c>
     </row>
     <row r="9">
@@ -847,7 +1029,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -860,13 +1042,13 @@
         <v>60</v>
       </c>
       <c r="G9" t="n">
-        <v>42252</v>
+        <v>40448</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9750544352930038</v>
+        <v>0.9680330300632911</v>
       </c>
       <c r="I9" t="n">
-        <v>0.882247793542621</v>
+        <v>0.7193401345778163</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
@@ -875,13 +1057,34 @@
         <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>0.969320331829428</v>
+        <v>0.9651801583454516</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9374406457739791</v>
+        <v>0.836763034970332</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9844211895471207</v>
+        <v>0.9822816032887975</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9681319224683544</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.7202083785543738</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.9652841368165903</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.8373501577287067</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.9823354483287882</v>
       </c>
     </row>
     <row r="10">
@@ -895,7 +1098,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -908,13 +1111,13 @@
         <v>120</v>
       </c>
       <c r="G10" t="n">
-        <v>41852</v>
+        <v>40286</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9706346172225939</v>
+        <v>0.9731420344536563</v>
       </c>
       <c r="I10" t="n">
-        <v>0.853847068616958</v>
+        <v>0.7539231294064135</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -923,13 +1126,34 @@
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>0.964553530226119</v>
+        <v>0.9707338183982041</v>
       </c>
       <c r="M10" t="n">
-        <v>0.9211623580730003</v>
+        <v>0.8596991701244814</v>
       </c>
       <c r="N10" t="n">
-        <v>0.9819569845114879</v>
+        <v>0.9851496019763931</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9732413245296133</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.7548328405731181</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.9708388562772202</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.8602903058579574</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.9852036894696387</v>
       </c>
     </row>
     <row r="11">
@@ -943,7 +1167,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -956,13 +1180,13 @@
         <v>180</v>
       </c>
       <c r="G11" t="n">
-        <v>41742</v>
+        <v>40041</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9733601648220018</v>
+        <v>0.9749506755575535</v>
       </c>
       <c r="I11" t="n">
-        <v>0.8666346845766371</v>
+        <v>0.766309412861137</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -971,13 +1195,34 @@
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.9677830571329239</v>
+        <v>0.9727089682194167</v>
       </c>
       <c r="M11" t="n">
-        <v>0.9285530711899255</v>
+        <v>0.8676955546761641</v>
       </c>
       <c r="N11" t="n">
-        <v>0.9836277974087161</v>
+        <v>0.9861657080591992</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.9750755475637471</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.7674743709226468</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.9728413203798949</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.8684418665963617</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.9862337232399029</v>
       </c>
     </row>
     <row r="12">
@@ -991,7 +1236,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1004,13 +1249,13 @@
         <v>240</v>
       </c>
       <c r="G12" t="n">
-        <v>41284</v>
+        <v>39852</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9681232438717179</v>
+        <v>0.9726738934056007</v>
       </c>
       <c r="I12" t="n">
-        <v>0.8365217391304348</v>
+        <v>0.7349720126551472</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
@@ -1019,13 +1264,34 @@
         <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9619102749638205</v>
+        <v>0.9704333188531712</v>
       </c>
       <c r="M12" t="n">
-        <v>0.9109848484848484</v>
+        <v>0.8472436526862113</v>
       </c>
       <c r="N12" t="n">
-        <v>0.980585388882332</v>
+        <v>0.9849948329314502</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.9727240790926428</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.7354587490873692</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.9704860168341026</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.8475669611555181</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.9850219778705579</v>
       </c>
     </row>
     <row r="13">
@@ -1039,7 +1305,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1052,13 +1318,13 @@
         <v>300</v>
       </c>
       <c r="G13" t="n">
-        <v>41355</v>
+        <v>39626</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9703058880425584</v>
+        <v>0.9689093019734518</v>
       </c>
       <c r="I13" t="n">
-        <v>0.8509889576507705</v>
+        <v>0.6984088127294982</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
@@ -1067,13 +1333,34 @@
         <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>0.964242035990915</v>
+        <v>0.9664971582411008</v>
       </c>
       <c r="M13" t="n">
-        <v>0.9194965255015078</v>
+        <v>0.8224272124531566</v>
       </c>
       <c r="N13" t="n">
-        <v>0.981795540796964</v>
+        <v>0.9829631883176149</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.9690354817544037</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.6996328029375765</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.966628590078329</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.82327524125018</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.9830311579471436</v>
       </c>
     </row>
     <row r="14">
@@ -1087,7 +1374,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1100,13 +1387,13 @@
         <v>30</v>
       </c>
       <c r="G14" t="n">
-        <v>42162</v>
+        <v>40497</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9798633840899388</v>
+        <v>0.9797268933501248</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8982136434480278</v>
+        <v>0.8183628318584071</v>
       </c>
       <c r="J14" t="n">
         <v>1</v>
@@ -1115,13 +1402,34 @@
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>0.9755119700028844</v>
+        <v>0.9776890048372194</v>
       </c>
       <c r="M14" t="n">
-        <v>0.946377818480389</v>
+        <v>0.9001095023725514</v>
       </c>
       <c r="N14" t="n">
-        <v>0.9876042107722183</v>
+        <v>0.988718653383717</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.979776279724424</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.8188053097345133</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.9777421458854223</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.9003770830799173</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.9887458260618636</v>
       </c>
     </row>
     <row r="15">
@@ -1135,7 +1443,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1148,13 +1456,13 @@
         <v>60</v>
       </c>
       <c r="G15" t="n">
-        <v>42269</v>
+        <v>40479</v>
       </c>
       <c r="H15" t="n">
-        <v>0.968038042063924</v>
+        <v>0.9761851824402776</v>
       </c>
       <c r="I15" t="n">
-        <v>0.850965250965251</v>
+        <v>0.7967531098460889</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
@@ -1163,13 +1471,34 @@
         <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>0.9609029084068875</v>
+        <v>0.9737329700272479</v>
       </c>
       <c r="M15" t="n">
-        <v>0.919482686691698</v>
+        <v>0.8868810138465149</v>
       </c>
       <c r="N15" t="n">
-        <v>0.980061689222096</v>
+        <v>0.9866917002595395</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.9761851824402776</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.7967531098460889</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>1</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.9737329700272479</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.8868810138465149</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.9866917002595395</v>
       </c>
     </row>
     <row r="16">
@@ -1183,7 +1512,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1196,13 +1525,13 @@
         <v>120</v>
       </c>
       <c r="G16" t="n">
-        <v>41803</v>
+        <v>40215</v>
       </c>
       <c r="H16" t="n">
-        <v>0.9687582230940364</v>
+        <v>0.9826432923038667</v>
       </c>
       <c r="I16" t="n">
-        <v>0.8425747348119575</v>
+        <v>0.8364573570759137</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
@@ -1211,13 +1540,34 @@
         <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9624852784879212</v>
+        <v>0.9809523809523809</v>
       </c>
       <c r="M16" t="n">
-        <v>0.9145623446290724</v>
+        <v>0.9109466700688951</v>
       </c>
       <c r="N16" t="n">
-        <v>0.980884074941452</v>
+        <v>0.9903846153846153</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.9827178913340793</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.8371602624179943</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.9810326947219038</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.9113633465119245</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.9904255465704169</v>
       </c>
     </row>
     <row r="17">
@@ -1231,7 +1581,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1244,13 +1594,13 @@
         <v>180</v>
       </c>
       <c r="G17" t="n">
-        <v>41653</v>
+        <v>39930</v>
       </c>
       <c r="H17" t="n">
-        <v>0.9757280387967253</v>
+        <v>0.9802153769095918</v>
       </c>
       <c r="I17" t="n">
-        <v>0.8724933787362845</v>
+        <v>0.8015573976387842</v>
       </c>
       <c r="J17" t="n">
         <v>1</v>
@@ -1259,13 +1609,34 @@
         <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>0.970893911040737</v>
+        <v>0.9784969650779826</v>
       </c>
       <c r="M17" t="n">
-        <v>0.9319054354415033</v>
+        <v>0.8898494143892917</v>
       </c>
       <c r="N17" t="n">
-        <v>0.9852320366934955</v>
+        <v>0.9891316310807836</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.9802404207362885</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.80180859080633</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.9785235995427078</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.8900041823504811</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.9891452391761938</v>
       </c>
     </row>
     <row r="18">
@@ -1279,7 +1650,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1292,13 +1663,13 @@
         <v>240</v>
       </c>
       <c r="G18" t="n">
-        <v>41271</v>
+        <v>39787</v>
       </c>
       <c r="H18" t="n">
-        <v>0.9755518402752538</v>
+        <v>0.9786613718048609</v>
       </c>
       <c r="I18" t="n">
-        <v>0.8748449516249069</v>
+        <v>0.7881736526946108</v>
       </c>
       <c r="J18" t="n">
         <v>1</v>
@@ -1307,13 +1678,34 @@
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>0.9705125957098603</v>
+        <v>0.9768210112482254</v>
       </c>
       <c r="M18" t="n">
-        <v>0.9332451207409859</v>
+        <v>0.8815403934700712</v>
       </c>
       <c r="N18" t="n">
-        <v>0.9850356682041318</v>
+        <v>0.9882746143328683</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.9786613718048609</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.7881736526946108</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.9768210112482254</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.8815403934700712</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.9882746143328683</v>
       </c>
     </row>
     <row r="19">
@@ -1327,7 +1719,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1340,13 +1732,13 @@
         <v>300</v>
       </c>
       <c r="G19" t="n">
-        <v>41112</v>
+        <v>39590</v>
       </c>
       <c r="H19" t="n">
-        <v>0.9647304923136797</v>
+        <v>0.9754736044455671</v>
       </c>
       <c r="I19" t="n">
-        <v>0.8190214677983025</v>
+        <v>0.7569461827284105</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>
@@ -1355,13 +1747,34 @@
         <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>0.9580318379160637</v>
+        <v>0.9734452770333096</v>
       </c>
       <c r="M19" t="n">
-        <v>0.9005077535336902</v>
+        <v>0.8616612052999003</v>
       </c>
       <c r="N19" t="n">
-        <v>0.9785661492978567</v>
+        <v>0.9865439780490848</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.9754988633493307</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.7571964956195244</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.9734718993573089</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.8618233618233617</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.9865576496674058</v>
       </c>
     </row>
     <row r="20">
@@ -1375,7 +1788,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1388,13 +1801,13 @@
         <v>30</v>
       </c>
       <c r="G20" t="n">
-        <v>42317</v>
+        <v>40483</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9752109081456625</v>
+        <v>0.9819430378183435</v>
       </c>
       <c r="I20" t="n">
-        <v>0.882989403234802</v>
+        <v>0.8424229359775813</v>
       </c>
       <c r="J20" t="n">
         <v>1</v>
@@ -1403,13 +1816,34 @@
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>0.9695067003866167</v>
+        <v>0.9800136705399863</v>
       </c>
       <c r="M20" t="n">
-        <v>0.937859131568035</v>
+        <v>0.9144729144729145</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9845172907472732</v>
+        <v>0.9899059639045003</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.9819924412716449</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.8428540633757275</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.9800672627348044</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.9147268686396069</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.9899333029537264</v>
       </c>
     </row>
     <row r="21">
@@ -1423,7 +1857,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1436,13 +1870,13 @@
         <v>60</v>
       </c>
       <c r="G21" t="n">
-        <v>42121</v>
+        <v>40408</v>
       </c>
       <c r="H21" t="n">
-        <v>0.9674271740936825</v>
+        <v>0.9820085131657098</v>
       </c>
       <c r="I21" t="n">
-        <v>0.8416253030128131</v>
+        <v>0.8388741134751773</v>
       </c>
       <c r="J21" t="n">
         <v>1</v>
@@ -1451,13 +1885,34 @@
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>0.96060867068619</v>
+        <v>0.9801490866395435</v>
       </c>
       <c r="M21" t="n">
-        <v>0.9140027579290461</v>
+        <v>0.9123779679402193</v>
       </c>
       <c r="N21" t="n">
-        <v>0.9799086223055296</v>
+        <v>0.9899750410237317</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.9820332607404474</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.839095744680851</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.9801758505816176</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.9125090383224873</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.989988692462561</v>
       </c>
     </row>
     <row r="22">
@@ -1471,7 +1926,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1484,13 +1939,13 @@
         <v>120</v>
       </c>
       <c r="G22" t="n">
-        <v>41983</v>
+        <v>40248</v>
       </c>
       <c r="H22" t="n">
-        <v>0.970321320534502</v>
+        <v>0.9795517789703836</v>
       </c>
       <c r="I22" t="n">
-        <v>0.8566002992289101</v>
+        <v>0.8054833372725124</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -1499,13 +1954,34 @@
         <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>0.9639258830341633</v>
+        <v>0.9776601520086862</v>
       </c>
       <c r="M22" t="n">
-        <v>0.9227622117530374</v>
+        <v>0.8922633852598508</v>
       </c>
       <c r="N22" t="n">
-        <v>0.981631630155969</v>
+        <v>0.9887038994194105</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.9795517789703836</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.8054833372725124</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.9776601520086862</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0.8922633852598508</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.9887038994194105</v>
       </c>
     </row>
     <row r="23">
@@ -1519,7 +1995,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1532,13 +2008,13 @@
         <v>180</v>
       </c>
       <c r="G23" t="n">
-        <v>41802</v>
+        <v>40014</v>
       </c>
       <c r="H23" t="n">
-        <v>0.9728481890818621</v>
+        <v>0.9805568051182086</v>
       </c>
       <c r="I23" t="n">
-        <v>0.8701075761043717</v>
+        <v>0.8180542563143124</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
@@ -1547,13 +2023,34 @@
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0.9668118950846516</v>
+        <v>0.9786942710044911</v>
       </c>
       <c r="M23" t="n">
-        <v>0.9305428064377945</v>
+        <v>0.899922819655261</v>
       </c>
       <c r="N23" t="n">
-        <v>0.9831259384802937</v>
+        <v>0.9892324300384753</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.9805568051182086</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.8180542563143124</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0.9786942710044911</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.899922819655261</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0.9892324300384753</v>
       </c>
     </row>
     <row r="24">
@@ -1567,7 +2064,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1580,13 +2077,13 @@
         <v>240</v>
       </c>
       <c r="G24" t="n">
-        <v>41418</v>
+        <v>39768</v>
       </c>
       <c r="H24" t="n">
-        <v>0.9613211647109953</v>
+        <v>0.9795815731241199</v>
       </c>
       <c r="I24" t="n">
-        <v>0.8024904450745901</v>
+        <v>0.8058809466889792</v>
       </c>
       <c r="J24" t="n">
         <v>1</v>
@@ -1595,13 +2092,34 @@
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>0.9541092554928529</v>
+        <v>0.9776904689946974</v>
       </c>
       <c r="M24" t="n">
-        <v>0.8904240766073871</v>
+        <v>0.8925072809107757</v>
       </c>
       <c r="N24" t="n">
-        <v>0.9765157734255893</v>
+        <v>0.9887194020727404</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.9795815731241199</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.8058809466889792</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1</v>
+      </c>
+      <c r="R24" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.9776904689946974</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.8925072809107757</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.9887194020727404</v>
       </c>
     </row>
     <row r="25">
@@ -1615,7 +2133,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>srcip</t>
+          <t>dstip</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1628,13 +2146,13 @@
         <v>300</v>
       </c>
       <c r="G25" t="n">
-        <v>40989</v>
+        <v>39591</v>
       </c>
       <c r="H25" t="n">
-        <v>0.949157090926834</v>
+        <v>0.9762319719128084</v>
       </c>
       <c r="I25" t="n">
-        <v>0.7352305933172405</v>
+        <v>0.7713244228432564</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -1643,13 +2161,34 @@
         <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>0.9407988182489632</v>
+        <v>0.9741604195842601</v>
       </c>
       <c r="M25" t="n">
-        <v>0.8474154341777713</v>
+        <v>0.870901358211003</v>
       </c>
       <c r="N25" t="n">
-        <v>0.9694964871194379</v>
+        <v>0.9869111040017804</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.9762319719128084</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.7713244228432564</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1</v>
+      </c>
+      <c r="R25" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0.9741604195842601</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.870901358211003</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.9869111040017804</v>
       </c>
     </row>
     <row r="26">
@@ -1663,7 +2202,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1676,13 +2215,13 @@
         <v>30</v>
       </c>
       <c r="G26" t="n">
-        <v>40450</v>
+        <v>41902</v>
       </c>
       <c r="H26" t="n">
-        <v>0.9800741656365883</v>
+        <v>0.9164240370388048</v>
       </c>
       <c r="I26" t="n">
-        <v>0.8090047393364929</v>
+        <v>0.5620310155077539</v>
       </c>
       <c r="J26" t="n">
         <v>1</v>
@@ -1691,13 +2230,34 @@
         <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>0.9782373906469382</v>
+        <v>0.9063836612489307</v>
       </c>
       <c r="M26" t="n">
-        <v>0.8944197013361279</v>
+        <v>0.7196156925540432</v>
       </c>
       <c r="N26" t="n">
-        <v>0.9889989899817105</v>
+        <v>0.9508932327453234</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.9166626891317837</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.5632816408204102</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1</v>
+      </c>
+      <c r="R26" t="n">
+        <v>1</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0.9066260227819669</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.7206400000000001</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0.9510265903736116</v>
       </c>
     </row>
     <row r="27">
@@ -1711,7 +2271,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1724,13 +2284,13 @@
         <v>60</v>
       </c>
       <c r="G27" t="n">
-        <v>40410</v>
+        <v>42274</v>
       </c>
       <c r="H27" t="n">
-        <v>0.9760207869339272</v>
+        <v>0.9052845720773999</v>
       </c>
       <c r="I27" t="n">
-        <v>0.7881040892193308</v>
+        <v>0.5493021161638901</v>
       </c>
       <c r="J27" t="n">
         <v>1</v>
@@ -1739,13 +2299,34 @@
         <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>0.9736727707439005</v>
+        <v>0.8929239985024335</v>
       </c>
       <c r="M27" t="n">
-        <v>0.8814968814968815</v>
+        <v>0.7090961929671608</v>
       </c>
       <c r="N27" t="n">
-        <v>0.9866607931941137</v>
+        <v>0.9434335443037974</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.9054265032880731</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.54997748761819</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>1</v>
+      </c>
+      <c r="R27" t="n">
+        <v>1</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.8930672943190329</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.7096586782861293</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.94351352115064</v>
       </c>
     </row>
     <row r="28">
@@ -1759,7 +2340,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1772,13 +2353,13 @@
         <v>120</v>
       </c>
       <c r="G28" t="n">
-        <v>40289</v>
+        <v>41881</v>
       </c>
       <c r="H28" t="n">
-        <v>0.9778847824468218</v>
+        <v>0.9094816265132161</v>
       </c>
       <c r="I28" t="n">
-        <v>0.794889502762431</v>
+        <v>0.544241404183698</v>
       </c>
       <c r="J28" t="n">
         <v>1</v>
@@ -1787,13 +2368,34 @@
         <v>1</v>
       </c>
       <c r="L28" t="n">
-        <v>0.9758117059398415</v>
+        <v>0.8985115382556085</v>
       </c>
       <c r="M28" t="n">
-        <v>0.8857252789534437</v>
+        <v>0.7048657065005839</v>
       </c>
       <c r="N28" t="n">
-        <v>0.9877577939297344</v>
+        <v>0.9465431419828814</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.9096726439196772</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.5452031738398654</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>1</v>
+      </c>
+      <c r="R28" t="n">
+        <v>1</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.8987040111390778</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.7056718275888897</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.9466499316024765</v>
       </c>
     </row>
     <row r="29">
@@ -1807,7 +2409,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1820,13 +2422,13 @@
         <v>180</v>
       </c>
       <c r="G29" t="n">
-        <v>40087</v>
+        <v>41793</v>
       </c>
       <c r="H29" t="n">
-        <v>0.9789457929004416</v>
+        <v>0.90543870983179</v>
       </c>
       <c r="I29" t="n">
-        <v>0.8056195301704284</v>
+        <v>0.5370196813495782</v>
       </c>
       <c r="J29" t="n">
         <v>1</v>
@@ -1835,13 +2437,34 @@
         <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>0.9769329579928394</v>
+        <v>0.8937891370367385</v>
       </c>
       <c r="M29" t="n">
-        <v>0.8923469387755102</v>
+        <v>0.698780487804878</v>
       </c>
       <c r="N29" t="n">
-        <v>0.9883319047750713</v>
+        <v>0.9439162149121563</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.9056779843514464</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.538191190253046</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>1</v>
+      </c>
+      <c r="R29" t="n">
+        <v>1</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0.8940294093927256</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.6997715156130998</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.9440501873509708</v>
       </c>
     </row>
     <row r="30">
@@ -1855,7 +2478,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1868,13 +2491,13 @@
         <v>240</v>
       </c>
       <c r="G30" t="n">
-        <v>39819</v>
+        <v>41221</v>
       </c>
       <c r="H30" t="n">
-        <v>0.9787036339435947</v>
+        <v>0.9112588243856287</v>
       </c>
       <c r="I30" t="n">
-        <v>0.7876283496118207</v>
+        <v>0.5258587167854828</v>
       </c>
       <c r="J30" t="n">
         <v>1</v>
@@ -1883,13 +2506,34 @@
         <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>0.9768773518023668</v>
+        <v>0.9015714131955656</v>
       </c>
       <c r="M30" t="n">
-        <v>0.8811992154665172</v>
+        <v>0.6892626571525653</v>
       </c>
       <c r="N30" t="n">
-        <v>0.988303448275862</v>
+        <v>0.9482382906466676</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.9116227165765023</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.5278029812054439</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>1</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.9019354491372581</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.6909306863493679</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.9484396008775035</v>
       </c>
     </row>
     <row r="31">
@@ -1903,7 +2547,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1916,13 +2560,13 @@
         <v>300</v>
       </c>
       <c r="G31" t="n">
-        <v>39690</v>
+        <v>41422</v>
       </c>
       <c r="H31" t="n">
-        <v>0.9785084404132023</v>
+        <v>0.9083337356960069</v>
       </c>
       <c r="I31" t="n">
-        <v>0.8006077606358111</v>
+        <v>0.5437943049381233</v>
       </c>
       <c r="J31" t="n">
         <v>1</v>
@@ -1931,13 +2575,34 @@
         <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>0.9764786984695988</v>
+        <v>0.8970891153512576</v>
       </c>
       <c r="M31" t="n">
-        <v>0.8892639231468259</v>
+        <v>0.7044906218382754</v>
       </c>
       <c r="N31" t="n">
-        <v>0.9880993903204655</v>
+        <v>0.9457532680905778</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.9086958621022645</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.5455965397092395</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>1</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.8974539735907378</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.7060012437810945</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.9459559874249786</v>
       </c>
     </row>
     <row r="32">
@@ -1951,7 +2616,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1964,13 +2629,13 @@
         <v>30</v>
       </c>
       <c r="G32" t="n">
-        <v>40550</v>
+        <v>42044</v>
       </c>
       <c r="H32" t="n">
-        <v>0.9887053020961776</v>
+        <v>0.9404433450670726</v>
       </c>
       <c r="I32" t="n">
-        <v>0.8981316725978647</v>
+        <v>0.6964480543096133</v>
       </c>
       <c r="J32" t="n">
         <v>1</v>
@@ -1979,13 +2644,34 @@
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>0.9874561787905346</v>
+        <v>0.9310173833989918</v>
       </c>
       <c r="M32" t="n">
-        <v>0.9463323177876728</v>
+        <v>0.8210661712162355</v>
       </c>
       <c r="N32" t="n">
-        <v>0.9936885042581924</v>
+        <v>0.964276542928068</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.9405860527066883</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.6971754152018427</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>1</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.931171300250737</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.8215714285714285</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.9643590914279191</v>
       </c>
     </row>
     <row r="33">
@@ -1999,7 +2685,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -2012,13 +2698,13 @@
         <v>60</v>
       </c>
       <c r="G33" t="n">
-        <v>40448</v>
+        <v>42252</v>
       </c>
       <c r="H33" t="n">
-        <v>0.986600079113924</v>
+        <v>0.931458865852504</v>
       </c>
       <c r="I33" t="n">
-        <v>0.8823529411764706</v>
+        <v>0.6764607306446208</v>
       </c>
       <c r="J33" t="n">
         <v>1</v>
@@ -2027,13 +2713,34 @@
         <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>0.9851029326883435</v>
+        <v>0.9199933696162665</v>
       </c>
       <c r="M33" t="n">
-        <v>0.9375</v>
+        <v>0.8070105291216846</v>
       </c>
       <c r="N33" t="n">
-        <v>0.9924955693398317</v>
+        <v>0.9583297361075139</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.9316245384833854</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.6772427661713775</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>1</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.9201713180436585</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.8075667754612669</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.958426271027903</v>
       </c>
     </row>
     <row r="34">
@@ -2047,7 +2754,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -2060,13 +2767,13 @@
         <v>120</v>
       </c>
       <c r="G34" t="n">
-        <v>40286</v>
+        <v>41852</v>
       </c>
       <c r="H34" t="n">
-        <v>0.9907163778980291</v>
+        <v>0.9339099684602886</v>
       </c>
       <c r="I34" t="n">
-        <v>0.9149420059131226</v>
+        <v>0.6710667142347485</v>
       </c>
       <c r="J34" t="n">
         <v>1</v>
@@ -2075,13 +2782,34 @@
         <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>0.9896864572704961</v>
+        <v>0.923610152172112</v>
       </c>
       <c r="M34" t="n">
-        <v>0.9555819477434679</v>
+        <v>0.8031596925704527</v>
       </c>
       <c r="N34" t="n">
-        <v>0.99481649850316</v>
+        <v>0.9602882903577787</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.9339816496224792</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.6714234748483767</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>1</v>
+      </c>
+      <c r="R34" t="n">
+        <v>1</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.9236866817654532</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.8034151547491996</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.9603296529741991</v>
       </c>
     </row>
     <row r="35">
@@ -2095,7 +2823,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -2108,13 +2836,13 @@
         <v>180</v>
       </c>
       <c r="G35" t="n">
-        <v>40041</v>
+        <v>41742</v>
       </c>
       <c r="H35" t="n">
-        <v>0.9897604954921205</v>
+        <v>0.9368980882564324</v>
       </c>
       <c r="I35" t="n">
-        <v>0.9044734389561976</v>
+        <v>0.6840969057327896</v>
       </c>
       <c r="J35" t="n">
         <v>1</v>
@@ -2123,13 +2851,34 @@
         <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>0.9886611908515169</v>
+        <v>0.9269104833786559</v>
       </c>
       <c r="M35" t="n">
-        <v>0.9498409591387327</v>
+        <v>0.8124198832075203</v>
       </c>
       <c r="N35" t="n">
-        <v>0.9942982700116817</v>
+        <v>0.9620690648310821</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.9370657850606104</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.6849364355960662</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>1</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0.9270905609058866</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.8130116022492704</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.9621660545834233</v>
       </c>
     </row>
     <row r="36">
@@ -2143,7 +2892,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -2156,13 +2905,13 @@
         <v>240</v>
       </c>
       <c r="G36" t="n">
-        <v>39852</v>
+        <v>41284</v>
       </c>
       <c r="H36" t="n">
-        <v>0.9885074776673692</v>
+        <v>0.939661854471466</v>
       </c>
       <c r="I36" t="n">
-        <v>0.888537357021173</v>
+        <v>0.6905590062111802</v>
       </c>
       <c r="J36" t="n">
         <v>1</v>
@@ -2171,13 +2920,34 @@
         <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>0.9873484157896191</v>
+        <v>0.9302729181245626</v>
       </c>
       <c r="M36" t="n">
-        <v>0.940979381443299</v>
+        <v>0.8169593651260195</v>
       </c>
       <c r="N36" t="n">
-        <v>0.9936339375069498</v>
+        <v>0.9638770863846633</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.9397829667667862</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0.6911801242236025</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1</v>
+      </c>
+      <c r="R36" t="n">
+        <v>1</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0.9304031354983203</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0.8173938592625238</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0.9639469791455174</v>
       </c>
     </row>
     <row r="37">
@@ -2191,7 +2961,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -2204,13 +2974,13 @@
         <v>300</v>
       </c>
       <c r="G37" t="n">
-        <v>39626</v>
+        <v>41355</v>
       </c>
       <c r="H37" t="n">
-        <v>0.9868268308686217</v>
+        <v>0.9316890339741265</v>
       </c>
       <c r="I37" t="n">
-        <v>0.8722154222766217</v>
+        <v>0.657201795898556</v>
       </c>
       <c r="J37" t="n">
         <v>1</v>
@@ -2219,13 +2989,34 @@
         <v>1</v>
       </c>
       <c r="L37" t="n">
-        <v>0.9855253306713252</v>
+        <v>0.9213945852694844</v>
       </c>
       <c r="M37" t="n">
-        <v>0.9317468619246861</v>
+        <v>0.793146371823973</v>
       </c>
       <c r="N37" t="n">
-        <v>0.9927099044746104</v>
+        <v>0.9590893951023127</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.931809938338774</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.6578085183836913</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>1</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0.921522791784939</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0.7935880544576196</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0.9591588460201599</v>
       </c>
     </row>
     <row r="38">
@@ -2239,7 +3030,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -2252,13 +3043,13 @@
         <v>30</v>
       </c>
       <c r="G38" t="n">
-        <v>40497</v>
+        <v>42162</v>
       </c>
       <c r="H38" t="n">
-        <v>0.9878756451095143</v>
+        <v>0.9484606992078175</v>
       </c>
       <c r="I38" t="n">
-        <v>0.8913716814159292</v>
+        <v>0.7394796786956001</v>
       </c>
       <c r="J38" t="n">
         <v>1</v>
@@ -2267,13 +3058,34 @@
         <v>1</v>
       </c>
       <c r="L38" t="n">
-        <v>0.986536141274542</v>
+        <v>0.9396288270267267</v>
       </c>
       <c r="M38" t="n">
-        <v>0.9425663820329863</v>
+        <v>0.8502308911709974</v>
       </c>
       <c r="N38" t="n">
-        <v>0.9932224446131549</v>
+        <v>0.9688748836209984</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0.948531853327641</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0.739839347800024</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>1</v>
+      </c>
+      <c r="R38" t="n">
+        <v>1</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0.9397071490094746</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0.8504685777287763</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0.9689165186500888</v>
       </c>
     </row>
     <row r="39">
@@ -2287,7 +3099,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -2300,13 +3112,13 @@
         <v>60</v>
       </c>
       <c r="G39" t="n">
-        <v>40479</v>
+        <v>42269</v>
       </c>
       <c r="H39" t="n">
-        <v>0.9880431828849527</v>
+        <v>0.9379450661241099</v>
       </c>
       <c r="I39" t="n">
-        <v>0.897954880877082</v>
+        <v>0.7106453392167678</v>
       </c>
       <c r="J39" t="n">
         <v>1</v>
@@ -2315,13 +3127,34 @@
         <v>1</v>
       </c>
       <c r="L39" t="n">
-        <v>0.9866372170071783</v>
+        <v>0.9267870600385184</v>
       </c>
       <c r="M39" t="n">
-        <v>0.9462341701844035</v>
+        <v>0.830850583607403</v>
       </c>
       <c r="N39" t="n">
-        <v>0.9932736672410917</v>
+        <v>0.9620025785516652</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0.938087014123826</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0.7113072255929399</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>1</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0.9269422964183021</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0.8313027783149616</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0.9620862006519377</v>
       </c>
     </row>
     <row r="40">
@@ -2335,7 +3168,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -2348,13 +3181,13 @@
         <v>120</v>
       </c>
       <c r="G40" t="n">
-        <v>40215</v>
+        <v>41803</v>
       </c>
       <c r="H40" t="n">
-        <v>0.9915205768991669</v>
+        <v>0.9396215582613688</v>
       </c>
       <c r="I40" t="n">
-        <v>0.9201030927835051</v>
+        <v>0.6957569913211186</v>
       </c>
       <c r="J40" t="n">
         <v>1</v>
@@ -2363,13 +3196,34 @@
         <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>0.9906029541446209</v>
+        <v>0.9299492104021537</v>
       </c>
       <c r="M40" t="n">
-        <v>0.9583892617449665</v>
+        <v>0.8205857264714245</v>
       </c>
       <c r="N40" t="n">
-        <v>0.9952792967398076</v>
+        <v>0.9637032989157008</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.9396454799894745</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0.695877531340405</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>1</v>
+      </c>
+      <c r="R40" t="n">
+        <v>1</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0.9299750208159867</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0.8206695571824579</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0.9637171577721213</v>
       </c>
     </row>
     <row r="41">
@@ -2383,7 +3237,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -2396,13 +3250,13 @@
         <v>180</v>
       </c>
       <c r="G41" t="n">
-        <v>39930</v>
+        <v>41653</v>
       </c>
       <c r="H41" t="n">
-        <v>0.9881793137991485</v>
+        <v>0.9412047151465681</v>
       </c>
       <c r="I41" t="n">
-        <v>0.8814368249183622</v>
+        <v>0.691133812586707</v>
       </c>
       <c r="J41" t="n">
         <v>1</v>
@@ -2411,13 +3265,34 @@
         <v>1</v>
       </c>
       <c r="L41" t="n">
-        <v>0.9870404437000632</v>
+        <v>0.9322975700107815</v>
       </c>
       <c r="M41" t="n">
-        <v>0.9369826435246996</v>
+        <v>0.8173614736371094</v>
       </c>
       <c r="N41" t="n">
-        <v>0.9934779604808622</v>
+        <v>0.9649627308754311</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0.9412527308957338</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.6913860512044394</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>1</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0.9323491194603412</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0.8175378420699426</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0.9649903426568425</v>
       </c>
     </row>
     <row r="42">
@@ -2431,7 +3306,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -2444,13 +3319,13 @@
         <v>240</v>
       </c>
       <c r="G42" t="n">
-        <v>39787</v>
+        <v>41271</v>
       </c>
       <c r="H42" t="n">
-        <v>0.9883378993138462</v>
+        <v>0.9446827069855346</v>
       </c>
       <c r="I42" t="n">
-        <v>0.8842315369261478</v>
+        <v>0.7168196477300918</v>
       </c>
       <c r="J42" t="n">
         <v>1</v>
@@ -2459,13 +3334,34 @@
         <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>0.9871975277984715</v>
+        <v>0.9356756452158232</v>
       </c>
       <c r="M42" t="n">
-        <v>0.9385593220338984</v>
+        <v>0.8350552705729354</v>
       </c>
       <c r="N42" t="n">
-        <v>0.9935575240898614</v>
+        <v>0.9667690426631345</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.9446827069855346</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0.7168196477300918</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>1</v>
+      </c>
+      <c r="R42" t="n">
+        <v>1</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0.9356756452158232</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0.8350552705729354</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0.9667690426631345</v>
       </c>
     </row>
     <row r="43">
@@ -2479,7 +3375,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -2492,13 +3388,13 @@
         <v>300</v>
       </c>
       <c r="G43" t="n">
-        <v>39590</v>
+        <v>41112</v>
       </c>
       <c r="H43" t="n">
-        <v>0.9863096741601415</v>
+        <v>0.9403823701109165</v>
       </c>
       <c r="I43" t="n">
-        <v>0.8643304130162703</v>
+        <v>0.694083874188717</v>
       </c>
       <c r="J43" t="n">
         <v>1</v>
@@ -2507,13 +3403,34 @@
         <v>1</v>
       </c>
       <c r="L43" t="n">
-        <v>0.9850015219857764</v>
+        <v>0.9310567916514303</v>
       </c>
       <c r="M43" t="n">
-        <v>0.9272287862513426</v>
+        <v>0.819420909157887</v>
       </c>
       <c r="N43" t="n">
-        <v>0.9924440974739308</v>
+        <v>0.9642976795676683</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.9404310177077252</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0.6943334997503744</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>1</v>
+      </c>
+      <c r="R43" t="n">
+        <v>1</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0.9311091732538187</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0.8195948434622468</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0.9643257731358068</v>
       </c>
     </row>
     <row r="44">
@@ -2527,7 +3444,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -2540,13 +3457,13 @@
         <v>30</v>
       </c>
       <c r="G44" t="n">
-        <v>40483</v>
+        <v>42317</v>
       </c>
       <c r="H44" t="n">
-        <v>0.9881925746609688</v>
+        <v>0.9473970271994706</v>
       </c>
       <c r="I44" t="n">
-        <v>0.8969605518430697</v>
+        <v>0.7517010596765198</v>
       </c>
       <c r="J44" t="n">
         <v>1</v>
@@ -2555,13 +3472,34 @@
         <v>1</v>
       </c>
       <c r="L44" t="n">
-        <v>0.9868399317218215</v>
+        <v>0.9374332452639271</v>
       </c>
       <c r="M44" t="n">
-        <v>0.9456818181818182</v>
+        <v>0.8582526744778399</v>
       </c>
       <c r="N44" t="n">
-        <v>0.9933763822298589</v>
+        <v>0.9677063687799217</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.9474206583642508</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0.7518126045733408</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>1</v>
+      </c>
+      <c r="R44" t="n">
+        <v>1</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0.9374595946819575</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0.8583253740846863</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0.9677204079560128</v>
       </c>
     </row>
     <row r="45">
@@ -2575,7 +3513,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2588,13 +3526,13 @@
         <v>60</v>
       </c>
       <c r="G45" t="n">
-        <v>40408</v>
+        <v>42121</v>
       </c>
       <c r="H45" t="n">
-        <v>0.9894327855870124</v>
+        <v>0.9441608698748842</v>
       </c>
       <c r="I45" t="n">
-        <v>0.905363475177305</v>
+        <v>0.7285005194505367</v>
       </c>
       <c r="J45" t="n">
         <v>1</v>
@@ -2603,13 +3541,34 @@
         <v>1</v>
       </c>
       <c r="L45" t="n">
-        <v>0.9882443630757372</v>
+        <v>0.9343200223401285</v>
       </c>
       <c r="M45" t="n">
-        <v>0.9503315109922066</v>
+        <v>0.8429277414184586</v>
       </c>
       <c r="N45" t="n">
-        <v>0.9940874285160415</v>
+        <v>0.9660449269503956</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0.9441608698748842</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.7285005194505367</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>1</v>
+      </c>
+      <c r="R45" t="n">
+        <v>1</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0.9343200223401285</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0.8429277414184586</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0.9660449269503956</v>
       </c>
     </row>
     <row r="46">
@@ -2623,7 +3582,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -2636,13 +3595,13 @@
         <v>120</v>
       </c>
       <c r="G46" t="n">
-        <v>40248</v>
+        <v>41983</v>
       </c>
       <c r="H46" t="n">
-        <v>0.9856141920095408</v>
+        <v>0.9447395374318176</v>
       </c>
       <c r="I46" t="n">
-        <v>0.8631529189316947</v>
+        <v>0.732995741742433</v>
       </c>
       <c r="J46" t="n">
         <v>1</v>
@@ -2651,13 +3610,34 @@
         <v>1</v>
       </c>
       <c r="L46" t="n">
-        <v>0.9841785987539622</v>
+        <v>0.9348570786769248</v>
       </c>
       <c r="M46" t="n">
-        <v>0.9265508055308893</v>
+        <v>0.8459290742462477</v>
       </c>
       <c r="N46" t="n">
-        <v>0.9920262212000606</v>
+        <v>0.9663319208219655</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0.9448109949265179</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.7333410058694901</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>1</v>
+      </c>
+      <c r="R46" t="n">
+        <v>1</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0.9349358344331807</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0.8461589535887392</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0.9663739931790146</v>
       </c>
     </row>
     <row r="47">
@@ -2671,7 +3651,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2684,13 +3664,13 @@
         <v>180</v>
       </c>
       <c r="G47" t="n">
-        <v>40014</v>
+        <v>41802</v>
       </c>
       <c r="H47" t="n">
-        <v>0.9826810616284301</v>
+        <v>0.9421319554088321</v>
       </c>
       <c r="I47" t="n">
-        <v>0.837932647333957</v>
+        <v>0.7231631952391852</v>
       </c>
       <c r="J47" t="n">
         <v>1</v>
@@ -2699,13 +3679,34 @@
         <v>1</v>
       </c>
       <c r="L47" t="n">
-        <v>0.9809777387389861</v>
+        <v>0.9318265084688442</v>
       </c>
       <c r="M47" t="n">
-        <v>0.9118208423463545</v>
+        <v>0.8393438267915255</v>
       </c>
       <c r="N47" t="n">
-        <v>0.9903975391095899</v>
+        <v>0.9647103447269756</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.9423233338117794</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0.7240787365529869</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>1</v>
+      </c>
+      <c r="R47" t="n">
+        <v>1</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0.9320366455250176</v>
+      </c>
+      <c r="T47" t="n">
+        <v>0.839960172585463</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0.9648229475189309</v>
       </c>
     </row>
     <row r="48">
@@ -2719,7 +3720,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -2732,13 +3733,13 @@
         <v>240</v>
       </c>
       <c r="G48" t="n">
-        <v>39768</v>
+        <v>41418</v>
       </c>
       <c r="H48" t="n">
-        <v>0.9843341380004024</v>
+        <v>0.9431406634796465</v>
       </c>
       <c r="I48" t="n">
-        <v>0.851063829787234</v>
+        <v>0.7096535568980397</v>
       </c>
       <c r="J48" t="n">
         <v>1</v>
@@ -2747,13 +3748,34 @@
         <v>1</v>
       </c>
       <c r="L48" t="n">
-        <v>0.9827938577110031</v>
+        <v>0.9339633223038528</v>
       </c>
       <c r="M48" t="n">
-        <v>0.9195402298850576</v>
+        <v>0.8301723516261629</v>
       </c>
       <c r="N48" t="n">
-        <v>0.9913222737592802</v>
+        <v>0.9658542243616697</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.94326138393935</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0.7102700036986808</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>1</v>
+      </c>
+      <c r="R48" t="n">
+        <v>1</v>
+      </c>
+      <c r="S48" t="n">
+        <v>0.9340942872367277</v>
+      </c>
+      <c r="T48" t="n">
+        <v>0.830594002306805</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0.9659242503335074</v>
       </c>
     </row>
     <row r="49">
@@ -2767,7 +3789,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>dstip</t>
+          <t>srcip</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2780,13 +3802,13 @@
         <v>300</v>
       </c>
       <c r="G49" t="n">
-        <v>39591</v>
+        <v>40989</v>
       </c>
       <c r="H49" t="n">
-        <v>0.981283625066303</v>
+        <v>0.9388128522286467</v>
       </c>
       <c r="I49" t="n">
-        <v>0.8199270959902795</v>
+        <v>0.6813619616313048</v>
       </c>
       <c r="J49" t="n">
         <v>1</v>
@@ -2795,13 +3817,34 @@
         <v>1</v>
       </c>
       <c r="L49" t="n">
-        <v>0.9795399950299583</v>
+        <v>0.9296019760848818</v>
       </c>
       <c r="M49" t="n">
-        <v>0.9010548804913873</v>
+        <v>0.8104881366178027</v>
       </c>
       <c r="N49" t="n">
-        <v>0.9896642628987488</v>
+        <v>0.963516816013034</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.9388372490180292</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0.6814890102909414</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>1</v>
+      </c>
+      <c r="R49" t="n">
+        <v>1</v>
+      </c>
+      <c r="S49" t="n">
+        <v>0.9296280701754386</v>
+      </c>
+      <c r="T49" t="n">
+        <v>0.8105780128447299</v>
+      </c>
+      <c r="U49" t="n">
+        <v>0.9635308322301908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>